<commit_message>
limpieza dataframe clientes y productos
</commit_message>
<xml_diff>
--- a/datasets/datasets_limpios/productos_limpio.xlsx
+++ b/datasets/datasets_limpios/productos_limpio.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -520,7 +520,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -556,7 +556,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -592,7 +592,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -628,7 +628,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -664,7 +664,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -700,7 +700,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -736,7 +736,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -772,7 +772,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -844,7 +844,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -916,7 +916,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -952,7 +952,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Limpieza</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Limpieza</t>
         </is>
       </c>
       <c r="D100" t="n">

</xml_diff>